<commit_message>
Resource new data and examine testcase scripts
</commit_message>
<xml_diff>
--- a/Data Files/Raw Data/Login Test.xlsx
+++ b/Data Files/Raw Data/Login Test.xlsx
@@ -141,20 +141,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,90 +171,91 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>